<commit_message>
red line is ready and blocks update with occupancy
</commit_message>
<xml_diff>
--- a/src/main/CTC/RedLine.xlsx
+++ b/src/main/CTC/RedLine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuliaCKoma\Documents\ECE-1140\src\main\CTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3EBB8DC2-546E-443E-8CEC-FFDE2312C86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E211888-2ED8-4894-B658-0302F27A8D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{79C304DD-ADC4-4B75-9259-2BA9FC0DDEDF}"/>
   </bookViews>
@@ -95,24 +95,12 @@
     <t>G</t>
   </si>
   <si>
-    <t>STATION; SWISSVILLE</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
-    <t>STATION; PENN STATION; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; FIRST AVE; UNDERGROUND</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
-    <t>STATION; STATION SQUARE</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -122,9 +110,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>STATION; SOUTH HILLS JUNCTION</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -152,19 +137,34 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>STATION; SHADYSIDE</t>
-  </si>
-  <si>
-    <t>STATION; HERRON AVE</t>
-  </si>
-  <si>
     <t>seconds to traverse block</t>
   </si>
   <si>
-    <t>STATION; STEEL PLAZA; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; YARD</t>
+    <t>YARD</t>
+  </si>
+  <si>
+    <t>SHADYSIDE</t>
+  </si>
+  <si>
+    <t>HERRON AVE</t>
+  </si>
+  <si>
+    <t>SWISSVILLE</t>
+  </si>
+  <si>
+    <t>PENN STATION</t>
+  </si>
+  <si>
+    <t>STEEL PLAZA</t>
+  </si>
+  <si>
+    <t>FIRST AVE</t>
+  </si>
+  <si>
+    <t>STATION SQUARE</t>
+  </si>
+  <si>
+    <t>SOUTH HILLS JUNCTION</t>
   </si>
 </sst>
 </file>
@@ -172,7 +172,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -205,7 +205,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113885C6-6377-4811-8022-2494B89DBA7F}">
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="E75" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,7 +571,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -594,7 +594,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="I2">
         <v>0.25</v>
@@ -603,7 +603,7 @@
         <v>0.25</v>
       </c>
       <c r="K2" s="1">
-        <f>D2/(F2/3.6)</f>
+        <f t="shared" ref="K2:K33" si="0">D2/(F2/3.6)</f>
         <v>4.5</v>
       </c>
     </row>
@@ -633,7 +633,7 @@
         <v>0.75</v>
       </c>
       <c r="K3" s="1">
-        <f>D3/(F3/3.6)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
@@ -663,7 +663,7 @@
         <v>1.5</v>
       </c>
       <c r="K4" s="1">
-        <f>D4/(F4/3.6)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
@@ -693,7 +693,7 @@
         <v>2.5</v>
       </c>
       <c r="K5" s="1">
-        <f>D5/(F5/3.6)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
@@ -723,7 +723,7 @@
         <v>3.25</v>
       </c>
       <c r="K6" s="1">
-        <f>D6/(F6/3.6)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
@@ -753,7 +753,7 @@
         <v>3.75</v>
       </c>
       <c r="K7" s="1">
-        <f>D7/(F7/3.6)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
@@ -777,7 +777,7 @@
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
@@ -789,7 +789,7 @@
         <v>4.13</v>
       </c>
       <c r="K8" s="1">
-        <f>D8/(F8/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
     </row>
@@ -819,7 +819,7 @@
         <v>4.13</v>
       </c>
       <c r="K9" s="1">
-        <f>D9/(F9/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
     </row>
@@ -849,7 +849,7 @@
         <v>4.13</v>
       </c>
       <c r="K10" s="1">
-        <f>D10/(F10/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
     </row>
@@ -879,7 +879,7 @@
         <v>4.13</v>
       </c>
       <c r="K11" s="1">
-        <f>D11/(F11/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
     </row>
@@ -909,7 +909,7 @@
         <v>3.75</v>
       </c>
       <c r="K12" s="1">
-        <f>D12/(F12/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
     </row>
@@ -939,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="1">
-        <f>D13/(F13/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
     </row>
@@ -969,7 +969,7 @@
         <v>1.6</v>
       </c>
       <c r="K14" s="1">
-        <f>D14/(F14/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.3</v>
       </c>
     </row>
@@ -999,7 +999,7 @@
         <v>0.85</v>
       </c>
       <c r="K15" s="1">
-        <f>D15/(F15/3.6)</f>
+        <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
         <v>0.25</v>
       </c>
       <c r="K16" s="1">
-        <f>D16/(F16/3.6)</f>
+        <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
         <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="1">
-        <f>D17/(F17/3.6)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
@@ -1095,7 +1095,7 @@
         <v>-1</v>
       </c>
       <c r="K18" s="1">
-        <f>D18/(F18/3.6)</f>
+        <f t="shared" si="0"/>
         <v>13.090909090909092</v>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
         <v>-1.24</v>
       </c>
       <c r="K19" s="1">
-        <f>D19/(F19/3.6)</f>
+        <f t="shared" si="0"/>
         <v>20.571428571428573</v>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
         <v>-1.24</v>
       </c>
       <c r="K20" s="1">
-        <f>D20/(F20/3.6)</f>
+        <f t="shared" si="0"/>
         <v>20.571428571428573</v>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
         <v>-1.24</v>
       </c>
       <c r="K21" s="1">
-        <f>D21/(F21/3.6)</f>
+        <f t="shared" si="0"/>
         <v>10.285714285714286</v>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
         <v>55</v>
       </c>
       <c r="G22" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
@@ -1221,7 +1221,7 @@
         <v>-1.24</v>
       </c>
       <c r="K22" s="1">
-        <f>D22/(F22/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.5454545454545459</v>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
         <v>-1.24</v>
       </c>
       <c r="K23" s="1">
-        <f>D23/(F23/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.5454545454545459</v>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
         <v>-1.24</v>
       </c>
       <c r="K24" s="1">
-        <f>D24/(F24/3.6)</f>
+        <f t="shared" si="0"/>
         <v>6.5454545454545459</v>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1311,7 +1311,7 @@
         <v>-1.24</v>
       </c>
       <c r="K25" s="1">
-        <f>D25/(F25/3.6)</f>
+        <f t="shared" si="0"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1335,7 +1335,7 @@
         <v>70</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H26" t="s">
         <v>14</v>
@@ -1347,7 +1347,7 @@
         <v>-1.24</v>
       </c>
       <c r="K26" s="1">
-        <f>D26/(F26/3.6)</f>
+        <f t="shared" si="0"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1377,7 +1377,7 @@
         <v>-1.24</v>
       </c>
       <c r="K27" s="1">
-        <f>D27/(F27/3.6)</f>
+        <f t="shared" si="0"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1407,7 +1407,7 @@
         <v>-1.24</v>
       </c>
       <c r="K28" s="1">
-        <f>D28/(F28/3.6)</f>
+        <f t="shared" si="0"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1437,7 +1437,7 @@
         <v>-1.24</v>
       </c>
       <c r="K29" s="1">
-        <f>D29/(F29/3.6)</f>
+        <f t="shared" si="0"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1446,7 +1446,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1467,7 +1467,7 @@
         <v>-1.24</v>
       </c>
       <c r="K30" s="1">
-        <f>D30/(F30/3.6)</f>
+        <f t="shared" si="0"/>
         <v>3.0857142857142859</v>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1497,7 +1497,7 @@
         <v>-1.24</v>
       </c>
       <c r="K31" s="1">
-        <f>D31/(F31/3.6)</f>
+        <f t="shared" si="0"/>
         <v>3.0857142857142859</v>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1527,7 +1527,7 @@
         <v>-1.24</v>
       </c>
       <c r="K32" s="1">
-        <f>D32/(F32/3.6)</f>
+        <f t="shared" si="0"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1557,7 +1557,7 @@
         <v>-1.24</v>
       </c>
       <c r="K33" s="1">
-        <f>D33/(F33/3.6)</f>
+        <f t="shared" si="0"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -1587,7 +1587,7 @@
         <v>-1.24</v>
       </c>
       <c r="K34" s="1">
-        <f>D34/(F34/3.6)</f>
+        <f t="shared" ref="K34:K65" si="1">D34/(F34/3.6)</f>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1596,7 +1596,7 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1617,7 +1617,7 @@
         <v>-1.24</v>
       </c>
       <c r="K35" s="1">
-        <f>D35/(F35/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1641,7 +1641,7 @@
         <v>70</v>
       </c>
       <c r="G36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H36" t="s">
         <v>14</v>
@@ -1653,7 +1653,7 @@
         <v>-1.24</v>
       </c>
       <c r="K36" s="1">
-        <f>D36/(F36/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1662,7 +1662,7 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1683,7 +1683,7 @@
         <v>-1.24</v>
       </c>
       <c r="K37" s="1">
-        <f>D37/(F37/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1692,7 +1692,7 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1713,7 +1713,7 @@
         <v>-1.24</v>
       </c>
       <c r="K38" s="1">
-        <f>D38/(F38/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1722,7 +1722,7 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1743,7 +1743,7 @@
         <v>-1.24</v>
       </c>
       <c r="K39" s="1">
-        <f>D39/(F39/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1752,7 +1752,7 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1773,7 +1773,7 @@
         <v>-1.24</v>
       </c>
       <c r="K40" s="1">
-        <f>D40/(F40/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1782,7 +1782,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1803,7 +1803,7 @@
         <v>-1.24</v>
       </c>
       <c r="K41" s="1">
-        <f>D41/(F41/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3.0857142857142859</v>
       </c>
     </row>
@@ -1812,7 +1812,7 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1833,7 +1833,7 @@
         <v>-1.24</v>
       </c>
       <c r="K42" s="1">
-        <f>D42/(F42/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3.0857142857142859</v>
       </c>
     </row>
@@ -1842,7 +1842,7 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1863,7 +1863,7 @@
         <v>-1.24</v>
       </c>
       <c r="K43" s="1">
-        <f>D43/(F43/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1872,7 +1872,7 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1893,7 +1893,7 @@
         <v>-1.24</v>
       </c>
       <c r="K44" s="1">
-        <f>D44/(F44/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1902,7 +1902,7 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1923,7 +1923,7 @@
         <v>-1.24</v>
       </c>
       <c r="K45" s="1">
-        <f>D45/(F45/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1932,7 +1932,7 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -1947,7 +1947,7 @@
         <v>70</v>
       </c>
       <c r="G46" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H46" t="s">
         <v>14</v>
@@ -1959,7 +1959,7 @@
         <v>-1.24</v>
       </c>
       <c r="K46" s="1">
-        <f>D46/(F46/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -1968,7 +1968,7 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1989,7 +1989,7 @@
         <v>-1.24</v>
       </c>
       <c r="K47" s="1">
-        <f>D47/(F47/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3.8571428571428577</v>
       </c>
     </row>
@@ -1998,7 +1998,7 @@
         <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -2019,7 +2019,7 @@
         <v>-1.24</v>
       </c>
       <c r="K48" s="1">
-        <f>D48/(F48/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3.8571428571428577</v>
       </c>
     </row>
@@ -2028,7 +2028,7 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -2043,7 +2043,7 @@
         <v>70</v>
       </c>
       <c r="G49" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="H49" t="s">
         <v>14</v>
@@ -2055,7 +2055,7 @@
         <v>-1.24</v>
       </c>
       <c r="K49" s="1">
-        <f>D49/(F49/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3.8571428571428577</v>
       </c>
     </row>
@@ -2064,7 +2064,7 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -2085,7 +2085,7 @@
         <v>-1.24</v>
       </c>
       <c r="K50" s="1">
-        <f>D50/(F50/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -2115,7 +2115,7 @@
         <v>-1.24</v>
       </c>
       <c r="K51" s="1">
-        <f>D51/(F51/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -2124,7 +2124,7 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C52">
         <v>51</v>
@@ -2145,7 +2145,7 @@
         <v>-1.24</v>
       </c>
       <c r="K52" s="1">
-        <f>D52/(F52/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C53">
         <v>52</v>
@@ -2175,7 +2175,7 @@
         <v>-1.24</v>
       </c>
       <c r="K53" s="1">
-        <f>D53/(F53/3.6)</f>
+        <f t="shared" si="1"/>
         <v>2.8276363636363642</v>
       </c>
     </row>
@@ -2184,7 +2184,7 @@
         <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C54">
         <v>53</v>
@@ -2205,7 +2205,7 @@
         <v>-1.24</v>
       </c>
       <c r="K54" s="1">
-        <f>D54/(F54/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2214,7 +2214,7 @@
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C55">
         <v>54</v>
@@ -2235,7 +2235,7 @@
         <v>-1.24</v>
       </c>
       <c r="K55" s="1">
-        <f>D55/(F55/3.6)</f>
+        <f t="shared" si="1"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2244,7 +2244,7 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C56">
         <v>55</v>
@@ -2265,7 +2265,7 @@
         <v>-0.87</v>
       </c>
       <c r="K56" s="1">
-        <f>D56/(F56/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C57">
         <v>56</v>
@@ -2295,7 +2295,7 @@
         <v>-0.49</v>
       </c>
       <c r="K57" s="1">
-        <f>D57/(F57/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2304,7 +2304,7 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C58">
         <v>57</v>
@@ -2325,7 +2325,7 @@
         <v>-0.12</v>
       </c>
       <c r="K58" s="1">
-        <f>D58/(F58/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2334,7 +2334,7 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -2355,7 +2355,7 @@
         <v>0.63</v>
       </c>
       <c r="K59" s="1">
-        <f>D59/(F59/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2364,7 +2364,7 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C60">
         <v>59</v>
@@ -2385,7 +2385,7 @@
         <v>1.01</v>
       </c>
       <c r="K60" s="1">
-        <f>D60/(F60/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2394,7 +2394,7 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -2409,7 +2409,7 @@
         <v>55</v>
       </c>
       <c r="G61" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="H61" t="s">
         <v>14</v>
@@ -2421,7 +2421,7 @@
         <v>1.01</v>
       </c>
       <c r="K61" s="1">
-        <f>D61/(F61/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2430,7 +2430,7 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C62">
         <v>61</v>
@@ -2451,7 +2451,7 @@
         <v>0.63</v>
       </c>
       <c r="K62" s="1">
-        <f>D62/(F62/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -2481,7 +2481,7 @@
         <v>-0.12</v>
       </c>
       <c r="K63" s="1">
-        <f>D63/(F63/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2490,7 +2490,7 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -2511,7 +2511,7 @@
         <v>-0.87</v>
       </c>
       <c r="K64" s="1">
-        <f>D64/(F64/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2520,7 +2520,7 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C65">
         <v>64</v>
@@ -2541,7 +2541,7 @@
         <v>-1.24</v>
       </c>
       <c r="K65" s="1">
-        <f>D65/(F65/3.6)</f>
+        <f t="shared" si="1"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2550,7 +2550,7 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C66">
         <v>65</v>
@@ -2571,7 +2571,7 @@
         <v>-1.24</v>
       </c>
       <c r="K66" s="1">
-        <f>D66/(F66/3.6)</f>
+        <f t="shared" ref="K66:K77" si="2">D66/(F66/3.6)</f>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2580,7 +2580,7 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C67">
         <v>66</v>
@@ -2601,7 +2601,7 @@
         <v>-1.24</v>
       </c>
       <c r="K67" s="1">
-        <f>D67/(F67/3.6)</f>
+        <f t="shared" si="2"/>
         <v>4.9090909090909092</v>
       </c>
     </row>
@@ -2610,7 +2610,7 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C68">
         <v>67</v>
@@ -2631,7 +2631,7 @@
         <v>-1.24</v>
       </c>
       <c r="K68" s="1">
-        <f>D68/(F68/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2640,7 +2640,7 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -2661,7 +2661,7 @@
         <v>-1.24</v>
       </c>
       <c r="K69" s="1">
-        <f>D69/(F69/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2670,7 +2670,7 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C70">
         <v>69</v>
@@ -2691,7 +2691,7 @@
         <v>-1.24</v>
       </c>
       <c r="K70" s="1">
-        <f>D70/(F70/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2700,7 +2700,7 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C71">
         <v>70</v>
@@ -2721,7 +2721,7 @@
         <v>-1.24</v>
       </c>
       <c r="K71" s="1">
-        <f>D71/(F71/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2730,7 +2730,7 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C72">
         <v>71</v>
@@ -2751,7 +2751,7 @@
         <v>-1.24</v>
       </c>
       <c r="K72" s="1">
-        <f>D72/(F72/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2760,7 +2760,7 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C73">
         <v>72</v>
@@ -2781,7 +2781,7 @@
         <v>-1.24</v>
       </c>
       <c r="K73" s="1">
-        <f>D73/(F73/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2790,7 +2790,7 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C74">
         <v>73</v>
@@ -2811,7 +2811,7 @@
         <v>-1.24</v>
       </c>
       <c r="K74" s="1">
-        <f>D74/(F74/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2820,7 +2820,7 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C75">
         <v>74</v>
@@ -2841,7 +2841,7 @@
         <v>-1.24</v>
       </c>
       <c r="K75" s="1">
-        <f>D75/(F75/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2850,7 +2850,7 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C76">
         <v>75</v>
@@ -2871,7 +2871,7 @@
         <v>-1.24</v>
       </c>
       <c r="K76" s="1">
-        <f>D76/(F76/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -2880,7 +2880,7 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C77">
         <v>76</v>
@@ -2901,393 +2901,393 @@
         <v>-1.24</v>
       </c>
       <c r="K77" s="1">
-        <f>D77/(F77/3.6)</f>
+        <f t="shared" si="2"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>